<commit_message>
chore: Add helper functions for calculating weeks and weekends in a month
</commit_message>
<xml_diff>
--- a/public/Template-Absensi.xlsx
+++ b/public/Template-Absensi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naufa\Desktop\Project\absensi-desa\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D6F173-7318-4533-80A9-9802E94374D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2FAF84-C31F-4499-B028-7296AE5E4C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="18220" xr2:uid="{D5544472-DC13-4845-9AB8-0E2AE791307A}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,13 +59,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF94DCF8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -95,9 +109,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -106,6 +123,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF94DCF8"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -437,7 +459,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,7 +469,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -458,7 +480,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
+      <c r="A2" s="2"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>

</xml_diff>